<commit_message>
Final changes of today, CO_f1ecac still not giving correct results
</commit_message>
<xml_diff>
--- a/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
+++ b/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
@@ -548,7 +548,7 @@
         <v>-0.2172266840934753</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>2.245543360870552</v>
+        <v>2.245543360870478</v>
       </c>
       <c r="D2" t="n">
         <v>6</v>
@@ -616,7 +616,7 @@
         <v>-0.2147622108459473</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>3.30560182848139</v>
+        <v>3.30560182848101</v>
       </c>
       <c r="D3" t="n">
         <v>8</v>
@@ -684,7 +684,7 @@
         <v>-0.08585639297962189</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.826515920865101</v>
+        <v>1.826515920865064</v>
       </c>
       <c r="D4" t="n">
         <v>5</v>
@@ -752,7 +752,7 @@
         <v>-0.4500797390937805</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>3.228657949064482</v>
+        <v>3.228657949064056</v>
       </c>
       <c r="D5" t="n">
         <v>10</v>
@@ -820,7 +820,7 @@
         <v>0.5725660920143127</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>3.412123258519425</v>
+        <v>3.412123258519119</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
@@ -888,7 +888,7 @@
         <v>-0.3925162255764008</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>2.345145650431962</v>
+        <v>2.345145650431858</v>
       </c>
       <c r="D7" t="n">
         <v>6</v>
@@ -956,7 +956,7 @@
         <v>-0.142518475651741</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>2.111142837746482</v>
+        <v>2.111142837746413</v>
       </c>
       <c r="D8" t="n">
         <v>7</v>
@@ -1024,7 +1024,7 @@
         <v>-0.3359417021274567</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>3.699873979106004</v>
+        <v>3.699873979105761</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>8</v>
@@ -1092,7 +1092,7 @@
         <v>0.7052313685417175</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>3.670459794708516</v>
+        <v>3.670459794708263</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>8</v>
@@ -1160,7 +1160,7 @@
         <v>-0.1334540843963623</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>3.13942864799979</v>
+        <v>3.139428647999336</v>
       </c>
       <c r="D11" t="n">
         <v>10</v>
@@ -1228,7 +1228,7 @@
         <v>-0.3635061681270599</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>2.844096786204988</v>
+        <v>2.844096786204584</v>
       </c>
       <c r="D12" t="n">
         <v>8</v>
@@ -1296,7 +1296,7 @@
         <v>-1.514761924743652</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>3.101766260610601</v>
+        <v>3.101766260610153</v>
       </c>
       <c r="D13" t="n">
         <v>8</v>
@@ -1364,7 +1364,7 @@
         <v>0.5681732892990112</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>3.389178070572797</v>
+        <v>3.389178070572481</v>
       </c>
       <c r="D14" t="n">
         <v>8</v>
@@ -1432,7 +1432,7 @@
         <v>0.6141835153102875</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>3.396970569549581</v>
+        <v>3.396970569549217</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>8</v>
@@ -1500,7 +1500,7 @@
         <v>-0.4390748143196106</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>3.246445256389047</v>
+        <v>3.246445256388673</v>
       </c>
       <c r="D16" t="n">
         <v>8</v>
@@ -1568,7 +1568,7 @@
         <v>-0.4183956980705261</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>2.384560970775786</v>
+        <v>2.384560970775679</v>
       </c>
       <c r="D17" t="n">
         <v>6</v>
@@ -1636,7 +1636,7 @@
         <v>0.7695344835519791</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>3.514985837357467</v>
+        <v>3.514985837357224</v>
       </c>
       <c r="D18" t="n">
         <v>6</v>
@@ -1704,7 +1704,7 @@
         <v>-0.3625948131084442</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>3.58883024088062</v>
+        <v>3.588830240880397</v>
       </c>
       <c r="D19" t="n">
         <v>6</v>
@@ -1772,7 +1772,7 @@
         <v>-0.4143381118774414</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>3.280512040827453</v>
+        <v>3.280512040827034</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>10</v>
@@ -1840,7 +1840,7 @@
         <v>0.5762799978256226</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>3.676215314762602</v>
+        <v>3.676215314762354</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>8</v>
@@ -1908,7 +1908,7 @@
         <v>1.023428201675415</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>3.356710081026915</v>
+        <v>3.356710081026564</v>
       </c>
       <c r="D22" t="n">
         <v>8</v>
@@ -1976,7 +1976,7 @@
         <v>0.6457960605621338</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>2.949372144650483</v>
+        <v>2.949372144650085</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>8</v>
@@ -2044,7 +2044,7 @@
         <v>0.4680100083351135</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>3.140384506129366</v>
+        <v>3.140384506128961</v>
       </c>
       <c r="D24" t="n">
         <v>7</v>
@@ -2112,7 +2112,7 @@
         <v>-0.1740318139394124</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>3.478566781820565</v>
+        <v>3.478566781820282</v>
       </c>
       <c r="D25" t="n">
         <v>8</v>
@@ -2180,7 +2180,7 @@
         <v>0.3508234620094299</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>3.004643487294367</v>
+        <v>3.00464348729393</v>
       </c>
       <c r="D26" t="n">
         <v>7</v>
@@ -2248,7 +2248,7 @@
         <v>-0.3646472990512848</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>1.987323928389985</v>
+        <v>1.987323928389954</v>
       </c>
       <c r="D27" t="n">
         <v>6</v>
@@ -2316,7 +2316,7 @@
         <v>0.3304328322410583</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>3.071363883181896</v>
+        <v>3.071363883181471</v>
       </c>
       <c r="D28" t="n">
         <v>7</v>
@@ -2384,7 +2384,7 @@
         <v>1.2090744972229</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>2.919894663659638</v>
+        <v>2.919894663659235</v>
       </c>
       <c r="D29" t="n">
         <v>9</v>
@@ -2452,7 +2452,7 @@
         <v>0.3232825696468353</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>3.157133396011119</v>
+        <v>3.157133396010675</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>8</v>
@@ -2520,7 +2520,7 @@
         <v>0.3791253566741943</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>3.355576584204473</v>
+        <v>3.35557658420413</v>
       </c>
       <c r="D31" t="n">
         <v>8</v>
@@ -2588,7 +2588,7 @@
         <v>1.027211666107178</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>3.561573084822518</v>
+        <v>3.56157308482224</v>
       </c>
       <c r="D32" t="n">
         <v>8</v>
@@ -2656,7 +2656,7 @@
         <v>-0.7519186735153198</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>2.256248150817039</v>
+        <v>2.25624815081696</v>
       </c>
       <c r="D33" t="n">
         <v>5</v>
@@ -2724,7 +2724,7 @@
         <v>-1.377173662185669</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>3.02826646812225</v>
+        <v>3.02826646812178</v>
       </c>
       <c r="D34" t="n">
         <v>10</v>
@@ -2792,7 +2792,7 @@
         <v>-0.8767848014831543</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>3.448647572559086</v>
+        <v>3.448647572558811</v>
       </c>
       <c r="D35" t="n">
         <v>6</v>
@@ -2860,7 +2860,7 @@
         <v>0.1222102642059326</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>2.059448363936673</v>
+        <v>2.059448363936612</v>
       </c>
       <c r="D36" t="n">
         <v>6</v>
@@ -2928,7 +2928,7 @@
         <v>-1.35373067855835</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>3.322914692736637</v>
+        <v>3.322914692736227</v>
       </c>
       <c r="D37" t="n">
         <v>10</v>
@@ -2996,7 +2996,7 @@
         <v>0.06383097171783447</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>3.890404192759865</v>
+        <v>3.890404192759681</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>16</v>
@@ -3064,7 +3064,7 @@
         <v>0.005945734679698944</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>1.960944948771081</v>
+        <v>1.960944948771042</v>
       </c>
       <c r="D39" t="n">
         <v>6</v>
@@ -3132,7 +3132,7 @@
         <v>0.5940335988998413</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>3.502617908531668</v>
+        <v>3.502617908531362</v>
       </c>
       <c r="D40" t="n">
         <v>8</v>
@@ -3200,7 +3200,7 @@
         <v>0.2458418309688568</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>3.58212642291229</v>
+        <v>3.582126422911973</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>12</v>
@@ -3268,7 +3268,7 @@
         <v>-0.5533497830231985</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>2.90931474896152</v>
+        <v>2.909314748961238</v>
       </c>
       <c r="D42" t="n">
         <v>5</v>
@@ -3336,7 +3336,7 @@
         <v>-0.2013241052627563</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>3.055647580060249</v>
+        <v>3.05564758005983</v>
       </c>
       <c r="D43" t="n">
         <v>7</v>
@@ -3404,7 +3404,7 @@
         <v>-1.386887311935425</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>3.400548422567045</v>
+        <v>3.40054842256667</v>
       </c>
       <c r="D44" t="n">
         <v>9</v>
@@ -3472,7 +3472,7 @@
         <v>0.1232104301452637</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>2.072244402765016</v>
+        <v>2.072244402764951</v>
       </c>
       <c r="D45" t="n">
         <v>7</v>
@@ -3540,7 +3540,7 @@
         <v>-0.4117159843444824</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>3.374829200679346</v>
+        <v>3.374829200679033</v>
       </c>
       <c r="D46" t="n">
         <v>8</v>
@@ -3608,7 +3608,7 @@
         <v>-1.343757629394531</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>2.998131463415418</v>
+        <v>2.99813146341499</v>
       </c>
       <c r="D47" t="n">
         <v>9</v>
@@ -3676,7 +3676,7 @@
         <v>-0.5499176979064941</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>2.339796701540011</v>
+        <v>2.339796701539905</v>
       </c>
       <c r="D48" t="n">
         <v>5</v>
@@ -3744,7 +3744,7 @@
         <v>-0.3411079943180084</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>3.262997344743428</v>
+        <v>3.262997344743015</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>10</v>
@@ -3812,7 +3812,7 @@
         <v>-0.2267749011516571</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>2.469661127172979</v>
+        <v>2.46966112717284</v>
       </c>
       <c r="D50" t="n">
         <v>7</v>
@@ -3880,7 +3880,7 @@
         <v>-0.3633207678794861</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>1.972691541567914</v>
+        <v>1.972691541567886</v>
       </c>
       <c r="D51" t="n">
         <v>6</v>
@@ -3948,7 +3948,7 @@
         <v>0.6527048349380493</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>3.387388014395206</v>
+        <v>3.387388014394869</v>
       </c>
       <c r="D52" t="n">
         <v>8</v>
@@ -4016,7 +4016,7 @@
         <v>-0.08114497363567352</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>2.152874034028958</v>
+        <v>2.152874034028877</v>
       </c>
       <c r="D53" t="n">
         <v>7</v>
@@ -4084,7 +4084,7 @@
         <v>0.6170146465301514</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>3.057040802649662</v>
+        <v>3.057040802649207</v>
       </c>
       <c r="D54" t="n">
         <v>8</v>
@@ -4152,7 +4152,7 @@
         <v>-0.1821102797985077</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>1.990439510243164</v>
+        <v>1.990439510243127</v>
       </c>
       <c r="D55" t="n">
         <v>6</v>
@@ -4220,7 +4220,7 @@
         <v>-0.7950617522001266</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>2.076413323261392</v>
+        <v>2.076413323261349</v>
       </c>
       <c r="D56" t="n">
         <v>6</v>
@@ -4288,7 +4288,7 @@
         <v>-0.4745312929153442</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>3.379076572867782</v>
+        <v>3.379076572867401</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>8</v>
@@ -4356,7 +4356,7 @@
         <v>-0.621077224612236</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>3.072295837936831</v>
+        <v>3.072295837936365</v>
       </c>
       <c r="D58" t="n">
         <v>9</v>
@@ -4424,7 +4424,7 @@
         <v>0.9700087308883667</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>3.854777680991552</v>
+        <v>3.854777680991358</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>16</v>
@@ -4492,7 +4492,7 @@
         <v>-0.1767330850873675</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>2.998803481508856</v>
+        <v>2.998803481508547</v>
       </c>
       <c r="D60" t="n">
         <v>6</v>
@@ -4560,7 +4560,7 @@
         <v>-0.4562288522720337</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>1.837308766502794</v>
+        <v>1.837308766502761</v>
       </c>
       <c r="D61" t="n">
         <v>6</v>
@@ -4628,7 +4628,7 @@
         <v>-1.379035830497742</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>3.095129001671112</v>
+        <v>3.095129001670651</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>10</v>
@@ -4696,7 +4696,7 @@
         <v>1.000827193260193</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>3.684800708408118</v>
+        <v>3.68480070840787</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>8</v>
@@ -4764,7 +4764,7 @@
         <v>1.074292063713074</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>2.907311151616773</v>
+        <v>2.907311151616438</v>
       </c>
       <c r="D64" t="n">
         <v>7</v>
@@ -4832,7 +4832,7 @@
         <v>0.8525265455245972</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>3.28585977595341</v>
+        <v>3.285859775952992</v>
       </c>
       <c r="D65" t="n">
         <v>8</v>
@@ -4900,7 +4900,7 @@
         <v>0.7601801753044128</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>3.238479202448542</v>
+        <v>3.238479202448134</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>8</v>
@@ -4968,7 +4968,7 @@
         <v>-1.36204195022583</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>3.312365901247355</v>
+        <v>3.312365901246937</v>
       </c>
       <c r="D67" t="n">
         <v>9</v>
@@ -5036,7 +5036,7 @@
         <v>-0.7230163812637329</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>1.834861412456896</v>
+        <v>1.83486141245687</v>
       </c>
       <c r="D68" t="n">
         <v>6</v>

</xml_diff>

<commit_message>
Completely Fixed _FC_Local_Simple_mean3_stderr, however _co_f1.. has an autocorrelation error again
</commit_message>
<xml_diff>
--- a/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
+++ b/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
@@ -548,7 +548,7 @@
         <v>-0.2172266840934753</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>2.245543360870478</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
         <v>6</v>
@@ -562,8 +562,8 @@
       <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>5</v>
+      <c r="H2" t="n">
+        <v>8</v>
       </c>
       <c r="I2" t="n">
         <v>0.04000000000000001</v>
@@ -589,8 +589,8 @@
       <c r="P2" t="n">
         <v>0.4680519470663282</v>
       </c>
-      <c r="Q2" s="1" t="n">
-        <v>8</v>
+      <c r="Q2" t="n">
+        <v>5</v>
       </c>
       <c r="R2" s="1" t="n">
         <v>1.778747513382372</v>
@@ -604,8 +604,8 @@
       <c r="U2" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V2" s="1" t="n">
-        <v>0.83675541816258</v>
+      <c r="V2" t="n">
+        <v>0.8574191573061893</v>
       </c>
     </row>
     <row r="3">
@@ -616,7 +616,7 @@
         <v>-0.2147622108459473</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>3.30560182848101</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
         <v>8</v>
@@ -630,8 +630,8 @@
       <c r="G3" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H3" s="1" t="n">
-        <v>5</v>
+      <c r="H3" t="n">
+        <v>15</v>
       </c>
       <c r="I3" t="n">
         <v>0.1111111111111111</v>
@@ -657,8 +657,8 @@
       <c r="P3" t="n">
         <v>0.7027748523460556</v>
       </c>
-      <c r="Q3" s="1" t="n">
-        <v>15</v>
+      <c r="Q3" t="n">
+        <v>5</v>
       </c>
       <c r="R3" t="n">
         <v>1.73023804570537</v>
@@ -672,8 +672,8 @@
       <c r="U3" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V3" s="1" t="n">
-        <v>0.6661598584833751</v>
+      <c r="V3" t="n">
+        <v>0.6826107272137758</v>
       </c>
     </row>
     <row r="4">
@@ -684,7 +684,7 @@
         <v>-0.08585639297962189</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.826515920865064</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
         <v>5</v>
@@ -699,7 +699,7 @@
         <v>0.9130434782608695</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I4" t="n">
         <v>0.03401360544217687</v>
@@ -725,8 +725,8 @@
       <c r="P4" t="n">
         <v>0.3105674139582154</v>
       </c>
-      <c r="Q4" s="1" t="n">
-        <v>4</v>
+      <c r="Q4" t="n">
+        <v>5</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>1.836011552168369</v>
@@ -740,8 +740,8 @@
       <c r="U4" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V4" s="1" t="n">
-        <v>0.8650730109199346</v>
+      <c r="V4" t="n">
+        <v>0.8864360551857</v>
       </c>
     </row>
     <row r="5">
@@ -752,7 +752,7 @@
         <v>-0.4500797390937805</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>3.228657949064056</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
         <v>10</v>
@@ -766,8 +766,8 @@
       <c r="G5" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H5" s="1" t="n">
-        <v>6</v>
+      <c r="H5" t="n">
+        <v>13</v>
       </c>
       <c r="I5" t="n">
         <v>0.1111111111111111</v>
@@ -793,8 +793,8 @@
       <c r="P5" t="n">
         <v>0.804047159219282</v>
       </c>
-      <c r="Q5" s="1" t="n">
-        <v>13</v>
+      <c r="Q5" t="n">
+        <v>6</v>
       </c>
       <c r="R5" t="n">
         <v>1.605420035791506</v>
@@ -808,8 +808,8 @@
       <c r="U5" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V5" s="1" t="n">
-        <v>0.64830914455489</v>
+      <c r="V5" t="n">
+        <v>0.6643191885375342</v>
       </c>
     </row>
     <row r="6">
@@ -820,7 +820,7 @@
         <v>0.5725660920143127</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>3.412123258519119</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
@@ -834,8 +834,8 @@
       <c r="G6" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H6" s="1" t="n">
-        <v>6</v>
+      <c r="H6" t="n">
+        <v>16</v>
       </c>
       <c r="I6" t="n">
         <v>0.1111111111111111</v>
@@ -861,8 +861,8 @@
       <c r="P6" t="n">
         <v>0.6754849824949913</v>
       </c>
-      <c r="Q6" s="1" t="n">
-        <v>16</v>
+      <c r="Q6" t="n">
+        <v>6</v>
       </c>
       <c r="R6" t="n">
         <v>1.73023804570537</v>
@@ -876,8 +876,8 @@
       <c r="U6" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V6" s="1" t="n">
-        <v>0.6579459846693219</v>
+      <c r="V6" t="n">
+        <v>0.6741940111567349</v>
       </c>
     </row>
     <row r="7">
@@ -888,7 +888,7 @@
         <v>-0.3925162255764008</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>2.345145650431858</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
         <v>6</v>
@@ -944,8 +944,8 @@
       <c r="U7" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V7" s="1" t="n">
-        <v>0.7987001306267925</v>
+      <c r="V7" t="n">
+        <v>0.8184240915298243</v>
       </c>
     </row>
     <row r="8">
@@ -956,7 +956,7 @@
         <v>-0.142518475651741</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>2.111142837746413</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
         <v>7</v>
@@ -970,8 +970,8 @@
       <c r="G8" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H8" s="1" t="n">
-        <v>7</v>
+      <c r="H8" t="n">
+        <v>8</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>0.02666666666666668</v>
@@ -997,8 +997,8 @@
       <c r="P8" t="n">
         <v>0.5978962573702267</v>
       </c>
-      <c r="Q8" s="1" t="n">
-        <v>8</v>
+      <c r="Q8" t="n">
+        <v>7</v>
       </c>
       <c r="R8" s="1" t="n">
         <v>1.83902118125715</v>
@@ -1012,8 +1012,8 @@
       <c r="U8" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V8" s="1" t="n">
-        <v>0.8669421343245584</v>
+      <c r="V8" t="n">
+        <v>0.8883513367359682</v>
       </c>
     </row>
     <row r="9">
@@ -1024,7 +1024,7 @@
         <v>-0.3359417021274567</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>3.699873979105761</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>8</v>
@@ -1038,8 +1038,8 @@
       <c r="G9" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H9" s="1" t="n">
-        <v>5</v>
+      <c r="H9" t="n">
+        <v>15</v>
       </c>
       <c r="I9" t="n">
         <v>0.1111111111111111</v>
@@ -1065,8 +1065,8 @@
       <c r="P9" t="n">
         <v>0.7373254361100833</v>
       </c>
-      <c r="Q9" s="1" t="n">
-        <v>15</v>
+      <c r="Q9" t="n">
+        <v>5</v>
       </c>
       <c r="R9" t="n">
         <v>1.73023804570537</v>
@@ -1080,8 +1080,8 @@
       <c r="U9" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V9" s="1" t="n">
-        <v>0.6138210068641288</v>
+      <c r="V9" t="n">
+        <v>0.6289793636448475</v>
       </c>
     </row>
     <row r="10">
@@ -1092,7 +1092,7 @@
         <v>0.7052313685417175</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>3.670459794708263</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>8</v>
@@ -1106,8 +1106,8 @@
       <c r="G10" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H10" s="1" t="n">
-        <v>5</v>
+      <c r="H10" t="n">
+        <v>16</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -1133,8 +1133,8 @@
       <c r="P10" t="n">
         <v>0.7404830606197635</v>
       </c>
-      <c r="Q10" s="1" t="n">
-        <v>16</v>
+      <c r="Q10" t="n">
+        <v>5</v>
       </c>
       <c r="R10" t="n">
         <v>1.73023804570537</v>
@@ -1148,8 +1148,8 @@
       <c r="U10" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V10" s="1" t="n">
-        <v>0.6005775785608443</v>
+      <c r="V10" t="n">
+        <v>0.6154088878652204</v>
       </c>
     </row>
     <row r="11">
@@ -1160,7 +1160,7 @@
         <v>-0.1334540843963623</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>3.139428647999336</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
         <v>10</v>
@@ -1174,8 +1174,8 @@
       <c r="G11" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H11" s="1" t="n">
-        <v>4</v>
+      <c r="H11" t="n">
+        <v>13</v>
       </c>
       <c r="I11" t="n">
         <v>0.1111111111111111</v>
@@ -1201,8 +1201,8 @@
       <c r="P11" t="n">
         <v>0.8302763920018271</v>
       </c>
-      <c r="Q11" s="1" t="n">
-        <v>13</v>
+      <c r="Q11" t="n">
+        <v>4</v>
       </c>
       <c r="R11" t="n">
         <v>1.483611654966423</v>
@@ -1216,8 +1216,8 @@
       <c r="U11" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V11" s="1" t="n">
-        <v>0.6521309403572546</v>
+      <c r="V11" t="n">
+        <v>0.6682353638799723</v>
       </c>
     </row>
     <row r="12">
@@ -1228,7 +1228,7 @@
         <v>-0.3635061681270599</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>2.844096786204584</v>
+        <v>4</v>
       </c>
       <c r="D12" t="n">
         <v>8</v>
@@ -1242,8 +1242,8 @@
       <c r="G12" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H12" s="1" t="n">
-        <v>4</v>
+      <c r="H12" t="n">
+        <v>11</v>
       </c>
       <c r="I12" t="n">
         <v>0.1111111111111111</v>
@@ -1269,8 +1269,8 @@
       <c r="P12" t="n">
         <v>0.7186019519514407</v>
       </c>
-      <c r="Q12" s="1" t="n">
-        <v>11</v>
+      <c r="Q12" t="n">
+        <v>4</v>
       </c>
       <c r="R12" t="n">
         <v>1.911059049329703</v>
@@ -1284,8 +1284,8 @@
       <c r="U12" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V12" s="1" t="n">
-        <v>0.7370563993323642</v>
+      <c r="V12" t="n">
+        <v>0.7552580635694194</v>
       </c>
     </row>
     <row r="13">
@@ -1296,7 +1296,7 @@
         <v>-1.514761924743652</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>3.101766260610153</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
         <v>8</v>
@@ -1311,7 +1311,7 @@
         <v>0.9565217391304348</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I13" t="n">
         <v>0.1111111111111111</v>
@@ -1337,8 +1337,8 @@
       <c r="P13" t="n">
         <v>0.6788710458531927</v>
       </c>
-      <c r="Q13" s="1" t="n">
-        <v>17</v>
+      <c r="Q13" t="n">
+        <v>5</v>
       </c>
       <c r="R13" t="n">
         <v>1.790511713580148</v>
@@ -1352,8 +1352,8 @@
       <c r="U13" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V13" s="1" t="n">
-        <v>0.6983743624362077</v>
+      <c r="V13" t="n">
+        <v>0.7156207708092244</v>
       </c>
     </row>
     <row r="14">
@@ -1364,7 +1364,7 @@
         <v>0.5681732892990112</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>3.389178070572481</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
         <v>8</v>
@@ -1378,8 +1378,8 @@
       <c r="G14" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H14" s="1" t="n">
-        <v>6</v>
+      <c r="H14" t="n">
+        <v>15</v>
       </c>
       <c r="I14" t="n">
         <v>0.1111111111111111</v>
@@ -1405,8 +1405,8 @@
       <c r="P14" t="n">
         <v>0.6784647622519333</v>
       </c>
-      <c r="Q14" s="1" t="n">
-        <v>15</v>
+      <c r="Q14" t="n">
+        <v>6</v>
       </c>
       <c r="R14" t="n">
         <v>1.73023804570537</v>
@@ -1420,8 +1420,8 @@
       <c r="U14" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V14" s="1" t="n">
-        <v>0.6650094846093758</v>
+      <c r="V14" t="n">
+        <v>0.6814319447688442</v>
       </c>
     </row>
     <row r="15">
@@ -1432,7 +1432,7 @@
         <v>0.6141835153102875</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>3.396970569549217</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>8</v>
@@ -1447,7 +1447,7 @@
         <v>0.8260869565217391</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="I15" t="n">
         <v>0.1111111111111111</v>
@@ -1473,8 +1473,8 @@
       <c r="P15" t="n">
         <v>0.7637942340039413</v>
       </c>
-      <c r="Q15" s="1" t="n">
-        <v>16</v>
+      <c r="Q15" t="n">
+        <v>3</v>
       </c>
       <c r="R15" t="n">
         <v>1.665693703666284</v>
@@ -1488,8 +1488,8 @@
       <c r="U15" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V15" s="1" t="n">
-        <v>0.641250713759876</v>
+      <c r="V15" t="n">
+        <v>0.65708644925339</v>
       </c>
     </row>
     <row r="16">
@@ -1500,7 +1500,7 @@
         <v>-0.4390748143196106</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>3.246445256388673</v>
+        <v>4</v>
       </c>
       <c r="D16" t="n">
         <v>8</v>
@@ -1515,7 +1515,7 @@
         <v>0.8695652173913043</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I16" t="n">
         <v>0.1111111111111111</v>
@@ -1541,8 +1541,8 @@
       <c r="P16" t="n">
         <v>0.6834612805791206</v>
       </c>
-      <c r="Q16" s="1" t="n">
-        <v>16</v>
+      <c r="Q16" t="n">
+        <v>4</v>
       </c>
       <c r="R16" t="n">
         <v>1.73023804570537</v>
@@ -1556,8 +1556,8 @@
       <c r="U16" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V16" s="1" t="n">
-        <v>0.6684719718814343</v>
+      <c r="V16" t="n">
+        <v>0.6849799384292986</v>
       </c>
     </row>
     <row r="17">
@@ -1568,7 +1568,7 @@
         <v>-0.4183956980705261</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>2.384560970775679</v>
+        <v>3</v>
       </c>
       <c r="D17" t="n">
         <v>6</v>
@@ -1624,19 +1624,19 @@
       <c r="U17" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V17" s="1" t="n">
-        <v>0.7485155768993137</v>
+      <c r="V17" t="n">
+        <v>0.7670002264041113</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>-0.0836450606584549</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" t="n">
         <v>0.7695344835519791</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>3.514985837357224</v>
+        <v>4</v>
       </c>
       <c r="D18" t="n">
         <v>6</v>
@@ -1651,7 +1651,7 @@
         <v>0.9565217391304348</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I18" t="n">
         <v>0.1111111111111111</v>
@@ -1677,8 +1677,8 @@
       <c r="P18" t="n">
         <v>0.6190143854148003</v>
       </c>
-      <c r="Q18" s="1" t="n">
-        <v>8</v>
+      <c r="Q18" t="n">
+        <v>5</v>
       </c>
       <c r="R18" t="n">
         <v>1.778747513382372</v>
@@ -1692,8 +1692,8 @@
       <c r="U18" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V18" s="1" t="n">
-        <v>0.7044351695646405</v>
+      <c r="V18" t="n">
+        <v>0.7218312500339272</v>
       </c>
     </row>
     <row r="19">
@@ -1704,7 +1704,7 @@
         <v>-0.3625948131084442</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>3.588830240880397</v>
+        <v>4</v>
       </c>
       <c r="D19" t="n">
         <v>6</v>
@@ -1719,7 +1719,7 @@
         <v>0.8260869565217391</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I19" t="n">
         <v>0.1666666666666667</v>
@@ -1745,8 +1745,8 @@
       <c r="P19" t="n">
         <v>0.6217645988052942</v>
       </c>
-      <c r="Q19" s="1" t="n">
-        <v>7</v>
+      <c r="Q19" t="n">
+        <v>4</v>
       </c>
       <c r="R19" t="n">
         <v>1.714203171343286</v>
@@ -1760,8 +1760,8 @@
       <c r="U19" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V19" s="1" t="n">
-        <v>0.6885317715154339</v>
+      <c r="V19" t="n">
+        <v>0.7055351163517595</v>
       </c>
     </row>
     <row r="20">
@@ -1772,7 +1772,7 @@
         <v>-0.4143381118774414</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>3.280512040827034</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>10</v>
@@ -1787,7 +1787,7 @@
         <v>0.7826086956521739</v>
       </c>
       <c r="H20" s="1" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I20" t="n">
         <v>0.1111111111111111</v>
@@ -1813,8 +1813,8 @@
       <c r="P20" t="n">
         <v>0.8088382236805132</v>
       </c>
-      <c r="Q20" s="1" t="n">
-        <v>16</v>
+      <c r="Q20" t="n">
+        <v>5</v>
       </c>
       <c r="R20" t="n">
         <v>1.483611654966423</v>
@@ -1828,8 +1828,8 @@
       <c r="U20" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V20" s="1" t="n">
-        <v>0.6302777775694512</v>
+      <c r="V20" t="n">
+        <v>0.6458425355632602</v>
       </c>
     </row>
     <row r="21">
@@ -1840,7 +1840,7 @@
         <v>0.5762799978256226</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>3.676215314762354</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>8</v>
@@ -1854,8 +1854,8 @@
       <c r="G21" t="n">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H21" s="1" t="n">
-        <v>6</v>
+      <c r="H21" t="n">
+        <v>15</v>
       </c>
       <c r="I21" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -1881,8 +1881,8 @@
       <c r="P21" t="n">
         <v>0.7202343528225197</v>
       </c>
-      <c r="Q21" s="1" t="n">
-        <v>15</v>
+      <c r="Q21" t="n">
+        <v>6</v>
       </c>
       <c r="R21" t="n">
         <v>1.73023804570537</v>
@@ -1896,8 +1896,8 @@
       <c r="U21" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V21" s="1" t="n">
-        <v>0.6335793307294701</v>
+      <c r="V21" t="n">
+        <v>0.6492256208314514</v>
       </c>
     </row>
     <row r="22">
@@ -1908,7 +1908,7 @@
         <v>1.023428201675415</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>3.356710081026564</v>
+        <v>4</v>
       </c>
       <c r="D22" t="n">
         <v>8</v>
@@ -1922,8 +1922,8 @@
       <c r="G22" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H22" s="1" t="n">
-        <v>5</v>
+      <c r="H22" t="n">
+        <v>15</v>
       </c>
       <c r="I22" t="n">
         <v>0.1111111111111111</v>
@@ -1949,8 +1949,8 @@
       <c r="P22" t="n">
         <v>0.7093218955161197</v>
       </c>
-      <c r="Q22" s="1" t="n">
-        <v>15</v>
+      <c r="Q22" t="n">
+        <v>5</v>
       </c>
       <c r="R22" t="n">
         <v>1.790511713580148</v>
@@ -1964,8 +1964,8 @@
       <c r="U22" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V22" s="1" t="n">
-        <v>0.6511065600306005</v>
+      <c r="V22" t="n">
+        <v>0.667185686402688</v>
       </c>
     </row>
     <row r="23">
@@ -1976,7 +1976,7 @@
         <v>0.6457960605621338</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>2.949372144650085</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>8</v>
@@ -1991,7 +1991,7 @@
         <v>0.9130434782608695</v>
       </c>
       <c r="H23" s="1" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="I23" t="n">
         <v>0.1111111111111111</v>
@@ -2017,8 +2017,8 @@
       <c r="P23" t="n">
         <v>0.7978298655752953</v>
       </c>
-      <c r="Q23" s="1" t="n">
-        <v>16</v>
+      <c r="Q23" t="n">
+        <v>6</v>
       </c>
       <c r="R23" t="n">
         <v>1.483611654966423</v>
@@ -2032,8 +2032,8 @@
       <c r="U23" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V23" s="1" t="n">
-        <v>0.650165701616685</v>
+      <c r="V23" t="n">
+        <v>0.6662215934181749</v>
       </c>
     </row>
     <row r="24">
@@ -2044,7 +2044,7 @@
         <v>0.4680100083351135</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>3.140384506128961</v>
+        <v>4</v>
       </c>
       <c r="D24" t="n">
         <v>7</v>
@@ -2059,7 +2059,7 @@
         <v>0.8695652173913043</v>
       </c>
       <c r="H24" s="1" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I24" t="n">
         <v>0.1111111111111111</v>
@@ -2085,8 +2085,8 @@
       <c r="P24" t="n">
         <v>0.6923145921415631</v>
       </c>
-      <c r="Q24" s="1" t="n">
-        <v>17</v>
+      <c r="Q24" t="n">
+        <v>5</v>
       </c>
       <c r="R24" t="n">
         <v>1.790511713580148</v>
@@ -2100,8 +2100,8 @@
       <c r="U24" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V24" s="1" t="n">
-        <v>0.6634989640766628</v>
+      <c r="V24" t="n">
+        <v>0.6798841218158759</v>
       </c>
     </row>
     <row r="25">
@@ -2112,7 +2112,7 @@
         <v>-0.1740318139394124</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>3.478566781820282</v>
+        <v>4</v>
       </c>
       <c r="D25" t="n">
         <v>8</v>
@@ -2127,7 +2127,7 @@
         <v>0.9130434782608695</v>
       </c>
       <c r="H25" s="1" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I25" t="n">
         <v>0.1111111111111111</v>
@@ -2153,8 +2153,8 @@
       <c r="P25" t="n">
         <v>0.656506326906396</v>
       </c>
-      <c r="Q25" s="1" t="n">
-        <v>16</v>
+      <c r="Q25" t="n">
+        <v>4</v>
       </c>
       <c r="R25" t="n">
         <v>1.605420035791506</v>
@@ -2168,8 +2168,8 @@
       <c r="U25" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V25" s="1" t="n">
-        <v>0.6830557184245316</v>
+      <c r="V25" t="n">
+        <v>0.6999238317103339</v>
       </c>
     </row>
     <row r="26">
@@ -2180,7 +2180,7 @@
         <v>0.3508234620094299</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>3.00464348729393</v>
+        <v>4</v>
       </c>
       <c r="D26" t="n">
         <v>7</v>
@@ -2194,8 +2194,8 @@
       <c r="G26" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H26" s="1" t="n">
-        <v>5</v>
+      <c r="H26" t="n">
+        <v>16</v>
       </c>
       <c r="I26" t="n">
         <v>0.0625</v>
@@ -2221,8 +2221,8 @@
       <c r="P26" t="n">
         <v>0.6636836025590529</v>
       </c>
-      <c r="Q26" s="1" t="n">
-        <v>16</v>
+      <c r="Q26" t="n">
+        <v>5</v>
       </c>
       <c r="R26" t="n">
         <v>1.73023804570537</v>
@@ -2236,8 +2236,8 @@
       <c r="U26" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V26" s="1" t="n">
-        <v>0.6896461033058153</v>
+      <c r="V26" t="n">
+        <v>0.7066769666510576</v>
       </c>
     </row>
     <row r="27">
@@ -2248,7 +2248,7 @@
         <v>-0.3646472990512848</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>1.987323928389954</v>
+        <v>3</v>
       </c>
       <c r="D27" t="n">
         <v>6</v>
@@ -2262,8 +2262,8 @@
       <c r="G27" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H27" s="1" t="n">
-        <v>5</v>
+      <c r="H27" t="n">
+        <v>7</v>
       </c>
       <c r="I27" t="n">
         <v>0.04000000000000001</v>
@@ -2289,8 +2289,8 @@
       <c r="P27" t="n">
         <v>0.4337770710588943</v>
       </c>
-      <c r="Q27" s="1" t="n">
-        <v>7</v>
+      <c r="Q27" t="n">
+        <v>5</v>
       </c>
       <c r="R27" t="n">
         <v>1.83902118125715</v>
@@ -2304,8 +2304,8 @@
       <c r="U27" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V27" s="1" t="n">
-        <v>0.9075594004019465</v>
+      <c r="V27" t="n">
+        <v>0.9299716493102558</v>
       </c>
     </row>
     <row r="28">
@@ -2316,7 +2316,7 @@
         <v>0.3304328322410583</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>3.071363883181471</v>
+        <v>4</v>
       </c>
       <c r="D28" t="n">
         <v>7</v>
@@ -2330,8 +2330,8 @@
       <c r="G28" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H28" s="1" t="n">
-        <v>4</v>
+      <c r="H28" t="n">
+        <v>15</v>
       </c>
       <c r="I28" t="n">
         <v>0.1111111111111111</v>
@@ -2357,8 +2357,8 @@
       <c r="P28" t="n">
         <v>0.6743069499229292</v>
       </c>
-      <c r="Q28" s="1" t="n">
-        <v>15</v>
+      <c r="Q28" t="n">
+        <v>4</v>
       </c>
       <c r="R28" t="n">
         <v>1.73023804570537</v>
@@ -2372,19 +2372,19 @@
       <c r="U28" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V28" s="1" t="n">
-        <v>0.6843983003032706</v>
+      <c r="V28" t="n">
+        <v>0.7012995687514046</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>1.058463215827942</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" t="n">
         <v>1.2090744972229</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>2.919894663659235</v>
+        <v>4</v>
       </c>
       <c r="D29" t="n">
         <v>9</v>
@@ -2398,8 +2398,8 @@
       <c r="G29" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H29" s="1" t="n">
-        <v>5</v>
+      <c r="H29" t="n">
+        <v>12</v>
       </c>
       <c r="I29" t="n">
         <v>0.1111111111111111</v>
@@ -2425,8 +2425,8 @@
       <c r="P29" t="n">
         <v>0.8349861566943183</v>
       </c>
-      <c r="Q29" s="1" t="n">
-        <v>12</v>
+      <c r="Q29" t="n">
+        <v>5</v>
       </c>
       <c r="R29" t="n">
         <v>1.714203171343286</v>
@@ -2440,8 +2440,8 @@
       <c r="U29" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V29" s="1" t="n">
-        <v>0.6592202618662243</v>
+      <c r="V29" t="n">
+        <v>0.6754997567266193</v>
       </c>
     </row>
     <row r="30">
@@ -2452,7 +2452,7 @@
         <v>0.3232825696468353</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>3.157133396010675</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>8</v>
@@ -2467,7 +2467,7 @@
         <v>0.9130434782608695</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I30" t="n">
         <v>0.1111111111111111</v>
@@ -2493,8 +2493,8 @@
       <c r="P30" t="n">
         <v>0.7789099676396366</v>
       </c>
-      <c r="Q30" s="1" t="n">
-        <v>16</v>
+      <c r="Q30" t="n">
+        <v>5</v>
       </c>
       <c r="R30" t="n">
         <v>1.605420035791506</v>
@@ -2508,8 +2508,8 @@
       <c r="U30" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V30" s="1" t="n">
-        <v>0.6357230137414817</v>
+      <c r="V30" t="n">
+        <v>0.651422242259642</v>
       </c>
     </row>
     <row r="31">
@@ -2520,7 +2520,7 @@
         <v>0.3791253566741943</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>3.35557658420413</v>
+        <v>4</v>
       </c>
       <c r="D31" t="n">
         <v>8</v>
@@ -2535,7 +2535,7 @@
         <v>0.8260869565217391</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I31" t="n">
         <v>0.1111111111111111</v>
@@ -2561,8 +2561,8 @@
       <c r="P31" t="n">
         <v>0.6814860262368827</v>
       </c>
-      <c r="Q31" s="1" t="n">
-        <v>16</v>
+      <c r="Q31" t="n">
+        <v>4</v>
       </c>
       <c r="R31" t="n">
         <v>1.665693703666284</v>
@@ -2576,8 +2576,8 @@
       <c r="U31" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V31" s="1" t="n">
-        <v>0.6692841971169188</v>
+      <c r="V31" t="n">
+        <v>0.6858122216291865</v>
       </c>
     </row>
     <row r="32">
@@ -2588,7 +2588,7 @@
         <v>1.027211666107178</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>3.56157308482224</v>
+        <v>4</v>
       </c>
       <c r="D32" t="n">
         <v>8</v>
@@ -2602,8 +2602,8 @@
       <c r="G32" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H32" s="1" t="n">
-        <v>5</v>
+      <c r="H32" t="n">
+        <v>15</v>
       </c>
       <c r="I32" t="n">
         <v>0.1111111111111111</v>
@@ -2629,8 +2629,8 @@
       <c r="P32" t="n">
         <v>0.7112305104666558</v>
       </c>
-      <c r="Q32" s="1" t="n">
-        <v>15</v>
+      <c r="Q32" t="n">
+        <v>5</v>
       </c>
       <c r="R32" t="n">
         <v>1.73023804570537</v>
@@ -2644,8 +2644,8 @@
       <c r="U32" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V32" s="1" t="n">
-        <v>0.6403723036187963</v>
+      <c r="V32" t="n">
+        <v>0.6561863467065937</v>
       </c>
     </row>
     <row r="33">
@@ -2656,7 +2656,7 @@
         <v>-0.7519186735153198</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>2.25624815081696</v>
+        <v>3</v>
       </c>
       <c r="D33" t="n">
         <v>5</v>
@@ -2670,8 +2670,8 @@
       <c r="G33" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H33" s="1" t="n">
-        <v>6</v>
+      <c r="H33" t="n">
+        <v>5</v>
       </c>
       <c r="I33" s="1" t="n">
         <v>0.06666666666666668</v>
@@ -2697,8 +2697,8 @@
       <c r="P33" t="n">
         <v>0.39634075014939</v>
       </c>
-      <c r="Q33" s="1" t="n">
-        <v>5</v>
+      <c r="Q33" t="n">
+        <v>6</v>
       </c>
       <c r="R33" t="n">
         <v>1.885299500946812</v>
@@ -2712,8 +2712,8 @@
       <c r="U33" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V33" s="1" t="n">
-        <v>0.8174712223479225</v>
+      <c r="V33" t="n">
+        <v>0.8376587367987973</v>
       </c>
     </row>
     <row r="34">
@@ -2724,7 +2724,7 @@
         <v>-1.377173662185669</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>3.02826646812178</v>
+        <v>4</v>
       </c>
       <c r="D34" t="n">
         <v>10</v>
@@ -2738,8 +2738,8 @@
       <c r="G34" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H34" s="1" t="n">
-        <v>6</v>
+      <c r="H34" t="n">
+        <v>13</v>
       </c>
       <c r="I34" t="n">
         <v>0.1111111111111111</v>
@@ -2765,8 +2765,8 @@
       <c r="P34" t="n">
         <v>0.8486668508358579</v>
       </c>
-      <c r="Q34" s="1" t="n">
-        <v>13</v>
+      <c r="Q34" t="n">
+        <v>6</v>
       </c>
       <c r="R34" t="n">
         <v>1.483611654966423</v>
@@ -2780,8 +2780,8 @@
       <c r="U34" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V34" s="1" t="n">
-        <v>0.635935610366822</v>
+      <c r="V34" t="n">
+        <v>0.6516400889749291</v>
       </c>
     </row>
     <row r="35">
@@ -2792,7 +2792,7 @@
         <v>-0.8767848014831543</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>3.448647572558811</v>
+        <v>4</v>
       </c>
       <c r="D35" t="n">
         <v>6</v>
@@ -2807,7 +2807,7 @@
         <v>0.9565217391304348</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I35" t="n">
         <v>0.1111111111111111</v>
@@ -2833,8 +2833,8 @@
       <c r="P35" t="n">
         <v>0.6054045887584985</v>
       </c>
-      <c r="Q35" s="1" t="n">
-        <v>7</v>
+      <c r="Q35" t="n">
+        <v>4</v>
       </c>
       <c r="R35" t="n">
         <v>1.714203171343286</v>
@@ -2848,8 +2848,8 @@
       <c r="U35" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V35" s="1" t="n">
-        <v>0.7222017470467508</v>
+      <c r="V35" t="n">
+        <v>0.7400365745078062</v>
       </c>
     </row>
     <row r="36">
@@ -2860,7 +2860,7 @@
         <v>0.1222102642059326</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>2.059448363936612</v>
+        <v>3</v>
       </c>
       <c r="D36" t="n">
         <v>6</v>
@@ -2874,8 +2874,8 @@
       <c r="G36" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H36" s="1" t="n">
-        <v>5</v>
+      <c r="H36" t="n">
+        <v>7</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>0.04000000000000001</v>
@@ -2901,8 +2901,8 @@
       <c r="P36" t="n">
         <v>0.5705471799181075</v>
       </c>
-      <c r="Q36" s="1" t="n">
-        <v>7</v>
+      <c r="Q36" t="n">
+        <v>5</v>
       </c>
       <c r="R36" s="1" t="n">
         <v>1.813261632874258</v>
@@ -2916,8 +2916,8 @@
       <c r="U36" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V36" s="1" t="n">
-        <v>0.8744251823984155</v>
+      <c r="V36" t="n">
+        <v>0.8960191792551805</v>
       </c>
     </row>
     <row r="37">
@@ -2928,7 +2928,7 @@
         <v>-1.35373067855835</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>3.322914692736227</v>
+        <v>4</v>
       </c>
       <c r="D37" t="n">
         <v>10</v>
@@ -2943,7 +2943,7 @@
         <v>0.7826086956521739</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="I37" t="n">
         <v>0.1111111111111111</v>
@@ -2969,8 +2969,8 @@
       <c r="P37" t="n">
         <v>0.8204341074181251</v>
       </c>
-      <c r="Q37" s="1" t="n">
-        <v>16</v>
+      <c r="Q37" t="n">
+        <v>6</v>
       </c>
       <c r="R37" t="n">
         <v>1.605420035791506</v>
@@ -2984,8 +2984,8 @@
       <c r="U37" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V37" s="1" t="n">
-        <v>0.6291603062906093</v>
+      <c r="V37" t="n">
+        <v>0.6446974682455934</v>
       </c>
     </row>
     <row r="38">
@@ -2996,7 +2996,7 @@
         <v>0.06383097171783447</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>3.890404192759681</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>16</v>
@@ -3010,8 +3010,8 @@
       <c r="G38" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H38" s="1" t="n">
-        <v>4</v>
+      <c r="H38" t="n">
+        <v>15</v>
       </c>
       <c r="I38" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -3037,8 +3037,8 @@
       <c r="P38" t="n">
         <v>0.7641136498668536</v>
       </c>
-      <c r="Q38" s="1" t="n">
-        <v>15</v>
+      <c r="Q38" t="n">
+        <v>4</v>
       </c>
       <c r="R38" t="n">
         <v>1.790511713580148</v>
@@ -3052,8 +3052,8 @@
       <c r="U38" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V38" s="1" t="n">
-        <v>0.5868051223459461</v>
+      <c r="V38" t="n">
+        <v>0.6012963197891809</v>
       </c>
     </row>
     <row r="39">
@@ -3064,7 +3064,7 @@
         <v>0.005945734679698944</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>1.960944948771042</v>
+        <v>3</v>
       </c>
       <c r="D39" t="n">
         <v>6</v>
@@ -3078,8 +3078,8 @@
       <c r="G39" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H39" s="1" t="n">
-        <v>5</v>
+      <c r="H39" t="n">
+        <v>7</v>
       </c>
       <c r="I39" s="1" t="n">
         <v>0.02666666666666668</v>
@@ -3105,8 +3105,8 @@
       <c r="P39" t="n">
         <v>0.5202304725836779</v>
       </c>
-      <c r="Q39" s="1" t="n">
-        <v>7</v>
+      <c r="Q39" t="n">
+        <v>5</v>
       </c>
       <c r="R39" t="n">
         <v>1.73023804570537</v>
@@ -3120,8 +3120,8 @@
       <c r="U39" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V39" s="1" t="n">
-        <v>0.9329675001352364</v>
+      <c r="V39" t="n">
+        <v>0.9560072040126173</v>
       </c>
     </row>
     <row r="40">
@@ -3132,7 +3132,7 @@
         <v>0.5940335988998413</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>3.502617908531362</v>
+        <v>4</v>
       </c>
       <c r="D40" t="n">
         <v>8</v>
@@ -3147,7 +3147,7 @@
         <v>0.9130434782608695</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="I40" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -3173,8 +3173,8 @@
       <c r="P40" t="n">
         <v>0.6995154028463711</v>
       </c>
-      <c r="Q40" s="1" t="n">
-        <v>16</v>
+      <c r="Q40" t="n">
+        <v>6</v>
       </c>
       <c r="R40" t="n">
         <v>1.665693703666284</v>
@@ -3188,8 +3188,8 @@
       <c r="U40" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V40" s="1" t="n">
-        <v>0.6480806958215264</v>
+      <c r="V40" t="n">
+        <v>0.6640850982452019</v>
       </c>
     </row>
     <row r="41">
@@ -3200,7 +3200,7 @@
         <v>0.2458418309688568</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>3.582126422911973</v>
+        <v>4</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>12</v>
@@ -3214,8 +3214,8 @@
       <c r="G41" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H41" s="1" t="n">
-        <v>5</v>
+      <c r="H41" t="n">
+        <v>15</v>
       </c>
       <c r="I41" t="n">
         <v>0.1111111111111111</v>
@@ -3241,8 +3241,8 @@
       <c r="P41" t="n">
         <v>0.8315490457628903</v>
       </c>
-      <c r="Q41" s="1" t="n">
-        <v>15</v>
+      <c r="Q41" t="n">
+        <v>5</v>
       </c>
       <c r="R41" t="n">
         <v>1.605420035791506</v>
@@ -3256,8 +3256,8 @@
       <c r="U41" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V41" s="1" t="n">
-        <v>0.5901100887283176</v>
+      <c r="V41" t="n">
+        <v>0.6046829025695121</v>
       </c>
     </row>
     <row r="42">
@@ -3268,7 +3268,7 @@
         <v>-0.5533497830231985</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>2.909314748961238</v>
+        <v>3</v>
       </c>
       <c r="D42" t="n">
         <v>5</v>
@@ -3282,8 +3282,8 @@
       <c r="G42" t="n">
         <v>1</v>
       </c>
-      <c r="H42" s="1" t="n">
-        <v>5</v>
+      <c r="H42" t="n">
+        <v>6</v>
       </c>
       <c r="I42" t="n">
         <v>0.1041666666666667</v>
@@ -3309,8 +3309,8 @@
       <c r="P42" t="n">
         <v>0.4987382332235186</v>
       </c>
-      <c r="Q42" s="1" t="n">
-        <v>6</v>
+      <c r="Q42" t="n">
+        <v>5</v>
       </c>
       <c r="R42" t="n">
         <v>1.714203171343286</v>
@@ -3324,8 +3324,8 @@
       <c r="U42" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V42" s="1" t="n">
-        <v>0.8273935895550478</v>
+      <c r="V42" t="n">
+        <v>0.847826137624116</v>
       </c>
     </row>
     <row r="43">
@@ -3336,7 +3336,7 @@
         <v>-0.2013241052627563</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>3.05564758005983</v>
+        <v>4</v>
       </c>
       <c r="D43" t="n">
         <v>7</v>
@@ -3350,8 +3350,8 @@
       <c r="G43" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H43" s="1" t="n">
-        <v>5</v>
+      <c r="H43" t="n">
+        <v>15</v>
       </c>
       <c r="I43" t="n">
         <v>0.0625</v>
@@ -3377,8 +3377,8 @@
       <c r="P43" t="n">
         <v>0.6574177797632969</v>
       </c>
-      <c r="Q43" s="1" t="n">
-        <v>15</v>
+      <c r="Q43" t="n">
+        <v>5</v>
       </c>
       <c r="R43" t="n">
         <v>1.73023804570537</v>
@@ -3392,8 +3392,8 @@
       <c r="U43" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V43" s="1" t="n">
-        <v>0.6902736568580091</v>
+      <c r="V43" t="n">
+        <v>0.7073200176862909</v>
       </c>
     </row>
     <row r="44">
@@ -3404,7 +3404,7 @@
         <v>-1.386887311935425</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>3.40054842256667</v>
+        <v>4</v>
       </c>
       <c r="D44" t="n">
         <v>9</v>
@@ -3419,7 +3419,7 @@
         <v>0.9565217391304348</v>
       </c>
       <c r="H44" s="1" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I44" t="n">
         <v>0.1111111111111111</v>
@@ -3445,8 +3445,8 @@
       <c r="P44" t="n">
         <v>0.8321812764474428</v>
       </c>
-      <c r="Q44" s="1" t="n">
-        <v>16</v>
+      <c r="Q44" t="n">
+        <v>5</v>
       </c>
       <c r="R44" t="n">
         <v>1.483611654966423</v>
@@ -3460,8 +3460,8 @@
       <c r="U44" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V44" s="1" t="n">
-        <v>0.605031158695595</v>
+      <c r="V44" t="n">
+        <v>0.6199724495025251</v>
       </c>
     </row>
     <row r="45">
@@ -3472,7 +3472,7 @@
         <v>0.1232104301452637</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>2.072244402764951</v>
+        <v>3</v>
       </c>
       <c r="D45" t="n">
         <v>7</v>
@@ -3486,8 +3486,8 @@
       <c r="G45" t="n">
         <v>1</v>
       </c>
-      <c r="H45" s="1" t="n">
-        <v>5</v>
+      <c r="H45" t="n">
+        <v>9</v>
       </c>
       <c r="I45" s="1" t="n">
         <v>0.08000000000000002</v>
@@ -3513,8 +3513,8 @@
       <c r="P45" t="n">
         <v>0.543849356713797</v>
       </c>
-      <c r="Q45" s="1" t="n">
-        <v>9</v>
+      <c r="Q45" t="n">
+        <v>5</v>
       </c>
       <c r="R45" s="1" t="n">
         <v>1.548155997005509</v>
@@ -3528,8 +3528,8 @@
       <c r="U45" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V45" s="1" t="n">
-        <v>0.8506350837309871</v>
+      <c r="V45" t="n">
+        <v>0.8716415822789345</v>
       </c>
     </row>
     <row r="46">
@@ -3540,7 +3540,7 @@
         <v>-0.4117159843444824</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>3.374829200679033</v>
+        <v>4</v>
       </c>
       <c r="D46" t="n">
         <v>8</v>
@@ -3554,8 +3554,8 @@
       <c r="G46" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H46" s="1" t="n">
-        <v>4</v>
+      <c r="H46" t="n">
+        <v>15</v>
       </c>
       <c r="I46" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -3581,8 +3581,8 @@
       <c r="P46" t="n">
         <v>0.662297742741271</v>
       </c>
-      <c r="Q46" s="1" t="n">
-        <v>15</v>
+      <c r="Q46" t="n">
+        <v>4</v>
       </c>
       <c r="R46" t="n">
         <v>1.73023804570537</v>
@@ -3596,8 +3596,8 @@
       <c r="U46" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V46" s="1" t="n">
-        <v>0.6662679161478898</v>
+      <c r="V46" t="n">
+        <v>0.6827214533705925</v>
       </c>
     </row>
     <row r="47">
@@ -3608,7 +3608,7 @@
         <v>-1.343757629394531</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>2.99813146341499</v>
+        <v>4</v>
       </c>
       <c r="D47" t="n">
         <v>9</v>
@@ -3622,8 +3622,8 @@
       <c r="G47" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H47" s="1" t="n">
-        <v>5</v>
+      <c r="H47" t="n">
+        <v>13</v>
       </c>
       <c r="I47" t="n">
         <v>0.1111111111111111</v>
@@ -3649,8 +3649,8 @@
       <c r="P47" t="n">
         <v>0.8179327885082108</v>
       </c>
-      <c r="Q47" s="1" t="n">
-        <v>13</v>
+      <c r="Q47" t="n">
+        <v>5</v>
       </c>
       <c r="R47" t="n">
         <v>1.483611654966423</v>
@@ -3664,8 +3664,8 @@
       <c r="U47" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V47" s="1" t="n">
-        <v>0.6543345173352624</v>
+      <c r="V47" t="n">
+        <v>0.6704933583602372</v>
       </c>
     </row>
     <row r="48">
@@ -3676,7 +3676,7 @@
         <v>-0.5499176979064941</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>2.339796701539905</v>
+        <v>3</v>
       </c>
       <c r="D48" t="n">
         <v>5</v>
@@ -3732,8 +3732,8 @@
       <c r="U48" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V48" s="1" t="n">
-        <v>0.8271754651982959</v>
+      <c r="V48" t="n">
+        <v>0.8476026266696666</v>
       </c>
     </row>
     <row r="49">
@@ -3744,7 +3744,7 @@
         <v>-0.3411079943180084</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>3.262997344743015</v>
+        <v>4</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>10</v>
@@ -3759,7 +3759,7 @@
         <v>0.9130434782608695</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="I49" t="n">
         <v>0.1111111111111111</v>
@@ -3785,8 +3785,8 @@
       <c r="P49" t="n">
         <v>0.8115764439333524</v>
       </c>
-      <c r="Q49" s="1" t="n">
-        <v>16</v>
+      <c r="Q49" t="n">
+        <v>6</v>
       </c>
       <c r="R49" t="n">
         <v>1.483611654966423</v>
@@ -3800,8 +3800,8 @@
       <c r="U49" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V49" s="1" t="n">
-        <v>0.6275847342922503</v>
+      <c r="V49" t="n">
+        <v>0.6430829873760525</v>
       </c>
     </row>
     <row r="50">
@@ -3812,7 +3812,7 @@
         <v>-0.2267749011516571</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>2.46966112717284</v>
+        <v>3</v>
       </c>
       <c r="D50" t="n">
         <v>7</v>
@@ -3826,8 +3826,8 @@
       <c r="G50" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H50" s="1" t="n">
-        <v>4</v>
+      <c r="H50" t="n">
+        <v>5</v>
       </c>
       <c r="I50" t="n">
         <v>0.1041666666666667</v>
@@ -3853,8 +3853,8 @@
       <c r="P50" t="n">
         <v>0.4418276414378308</v>
       </c>
-      <c r="Q50" s="1" t="n">
-        <v>5</v>
+      <c r="Q50" t="n">
+        <v>4</v>
       </c>
       <c r="R50" s="1" t="n">
         <v>1.665693703666284</v>
@@ -3868,8 +3868,8 @@
       <c r="U50" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V50" s="1" t="n">
-        <v>0.7794775098306321</v>
+      <c r="V50" t="n">
+        <v>0.7987267666407276</v>
       </c>
     </row>
     <row r="51">
@@ -3880,7 +3880,7 @@
         <v>-0.3633207678794861</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>1.972691541567886</v>
+        <v>3</v>
       </c>
       <c r="D51" t="n">
         <v>6</v>
@@ -3894,8 +3894,8 @@
       <c r="G51" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H51" s="1" t="n">
-        <v>5</v>
+      <c r="H51" t="n">
+        <v>7</v>
       </c>
       <c r="I51" s="1" t="n">
         <v>0.04000000000000001</v>
@@ -3921,8 +3921,8 @@
       <c r="P51" t="n">
         <v>0.4280771712004225</v>
       </c>
-      <c r="Q51" s="1" t="n">
-        <v>7</v>
+      <c r="Q51" t="n">
+        <v>5</v>
       </c>
       <c r="R51" t="n">
         <v>1.548155997005509</v>
@@ -3936,8 +3936,8 @@
       <c r="U51" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V51" s="1" t="n">
-        <v>0.9128642833246349</v>
+      <c r="V51" t="n">
+        <v>0.9354075367230528</v>
       </c>
     </row>
     <row r="52">
@@ -3948,7 +3948,7 @@
         <v>0.6527048349380493</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>3.387388014394869</v>
+        <v>4</v>
       </c>
       <c r="D52" t="n">
         <v>8</v>
@@ -3963,7 +3963,7 @@
         <v>0.9130434782608695</v>
       </c>
       <c r="H52" s="1" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I52" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -3989,8 +3989,8 @@
       <c r="P52" t="n">
         <v>0.6796055464304638</v>
       </c>
-      <c r="Q52" s="1" t="n">
-        <v>16</v>
+      <c r="Q52" t="n">
+        <v>5</v>
       </c>
       <c r="R52" t="n">
         <v>1.548155997005509</v>
@@ -4004,8 +4004,8 @@
       <c r="U52" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V52" s="1" t="n">
-        <v>0.6672121894559961</v>
+      <c r="V52" t="n">
+        <v>0.6836890455803701</v>
       </c>
     </row>
     <row r="53">
@@ -4016,7 +4016,7 @@
         <v>-0.08114497363567352</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>2.152874034028877</v>
+        <v>3</v>
       </c>
       <c r="D53" t="n">
         <v>7</v>
@@ -4030,8 +4030,8 @@
       <c r="G53" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H53" s="1" t="n">
-        <v>6</v>
+      <c r="H53" t="n">
+        <v>7</v>
       </c>
       <c r="I53" s="1" t="n">
         <v>0.0625</v>
@@ -4057,8 +4057,8 @@
       <c r="P53" t="n">
         <v>0.5746041788589592</v>
       </c>
-      <c r="Q53" s="1" t="n">
-        <v>7</v>
+      <c r="Q53" t="n">
+        <v>6</v>
       </c>
       <c r="R53" t="n">
         <v>1.665693703666284</v>
@@ -4072,8 +4072,8 @@
       <c r="U53" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V53" s="1" t="n">
-        <v>0.8167532188690347</v>
+      <c r="V53" t="n">
+        <v>0.8369230021690024</v>
       </c>
     </row>
     <row r="54">
@@ -4084,7 +4084,7 @@
         <v>0.6170146465301514</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>3.057040802649207</v>
+        <v>4</v>
       </c>
       <c r="D54" t="n">
         <v>8</v>
@@ -4099,7 +4099,7 @@
         <v>1</v>
       </c>
       <c r="H54" s="1" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="I54" t="n">
         <v>0.1111111111111111</v>
@@ -4125,8 +4125,8 @@
       <c r="P54" t="n">
         <v>0.7815817352682647</v>
       </c>
-      <c r="Q54" s="1" t="n">
-        <v>16</v>
+      <c r="Q54" t="n">
+        <v>6</v>
       </c>
       <c r="R54" t="n">
         <v>1.639934155283393</v>
@@ -4140,8 +4140,8 @@
       <c r="U54" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V54" s="1" t="n">
-        <v>0.6290438955262714</v>
+      <c r="V54" t="n">
+        <v>0.6445781827085135</v>
       </c>
     </row>
     <row r="55">
@@ -4152,7 +4152,7 @@
         <v>-0.1821102797985077</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>1.990439510243127</v>
+        <v>3</v>
       </c>
       <c r="D55" t="n">
         <v>6</v>
@@ -4166,8 +4166,8 @@
       <c r="G55" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H55" s="1" t="n">
-        <v>5</v>
+      <c r="H55" t="n">
+        <v>7</v>
       </c>
       <c r="I55" s="1" t="n">
         <v>0.02666666666666668</v>
@@ -4193,8 +4193,8 @@
       <c r="P55" t="n">
         <v>0.5265412832179288</v>
       </c>
-      <c r="Q55" s="1" t="n">
-        <v>7</v>
+      <c r="Q55" t="n">
+        <v>5</v>
       </c>
       <c r="R55" t="n">
         <v>1.73023804570537</v>
@@ -4208,19 +4208,19 @@
       <c r="U55" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V55" s="1" t="n">
-        <v>0.9114871685485055</v>
+      <c r="V55" t="n">
+        <v>0.9339964139920454</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
+      <c r="A56" t="n">
         <v>0.03023050725460052</v>
       </c>
       <c r="B56" t="n">
         <v>-0.7950617522001266</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>2.076413323261349</v>
+        <v>3</v>
       </c>
       <c r="D56" t="n">
         <v>6</v>
@@ -4234,8 +4234,8 @@
       <c r="G56" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H56" s="1" t="n">
-        <v>5</v>
+      <c r="H56" t="n">
+        <v>8</v>
       </c>
       <c r="I56" s="1" t="n">
         <v>0.04000000000000001</v>
@@ -4261,8 +4261,8 @@
       <c r="P56" t="n">
         <v>0.441599982420937</v>
       </c>
-      <c r="Q56" s="1" t="n">
-        <v>8</v>
+      <c r="Q56" t="n">
+        <v>5</v>
       </c>
       <c r="R56" s="1" t="n">
         <v>1.778747513382372</v>
@@ -4276,8 +4276,8 @@
       <c r="U56" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V56" s="1" t="n">
-        <v>0.8859659347284118</v>
+      <c r="V56" t="n">
+        <v>0.907844931347941</v>
       </c>
     </row>
     <row r="57">
@@ -4288,7 +4288,7 @@
         <v>-0.4745312929153442</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>3.379076572867401</v>
+        <v>4</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>8</v>
@@ -4302,8 +4302,8 @@
       <c r="G57" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H57" s="1" t="n">
-        <v>4</v>
+      <c r="H57" t="n">
+        <v>15</v>
       </c>
       <c r="I57" t="n">
         <v>0.1111111111111111</v>
@@ -4329,8 +4329,8 @@
       <c r="P57" t="n">
         <v>0.7750123137142799</v>
       </c>
-      <c r="Q57" s="1" t="n">
-        <v>15</v>
+      <c r="Q57" t="n">
+        <v>4</v>
       </c>
       <c r="R57" t="n">
         <v>1.790511713580148</v>
@@ -4344,19 +4344,19 @@
       <c r="U57" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V57" s="1" t="n">
-        <v>0.6330814726579055</v>
+      <c r="V57" t="n">
+        <v>0.6487154681166755</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n">
+      <c r="A58" t="n">
         <v>0.4018734991550446</v>
       </c>
       <c r="B58" t="n">
         <v>-0.621077224612236</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>3.072295837936365</v>
+        <v>4</v>
       </c>
       <c r="D58" t="n">
         <v>9</v>
@@ -4371,7 +4371,7 @@
         <v>0.7826086956521739</v>
       </c>
       <c r="H58" s="1" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="I58" t="n">
         <v>0.1111111111111111</v>
@@ -4397,8 +4397,8 @@
       <c r="P58" t="n">
         <v>0.7963553909586716</v>
       </c>
-      <c r="Q58" s="1" t="n">
-        <v>16</v>
+      <c r="Q58" t="n">
+        <v>6</v>
       </c>
       <c r="R58" s="1" t="n">
         <v>1.73023804570537</v>
@@ -4412,8 +4412,8 @@
       <c r="U58" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V58" s="1" t="n">
-        <v>0.6452642671077279</v>
+      <c r="V58" t="n">
+        <v>0.6611991176085891</v>
       </c>
     </row>
     <row r="59">
@@ -4424,7 +4424,7 @@
         <v>0.9700087308883667</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>3.854777680991358</v>
+        <v>4</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>16</v>
@@ -4438,8 +4438,8 @@
       <c r="G59" t="n">
         <v>1</v>
       </c>
-      <c r="H59" s="1" t="n">
-        <v>5</v>
+      <c r="H59" t="n">
+        <v>15</v>
       </c>
       <c r="I59" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -4465,8 +4465,8 @@
       <c r="P59" t="n">
         <v>0.7561383689918901</v>
       </c>
-      <c r="Q59" s="1" t="n">
-        <v>15</v>
+      <c r="Q59" t="n">
+        <v>5</v>
       </c>
       <c r="R59" t="n">
         <v>1.790511713580148</v>
@@ -4480,8 +4480,8 @@
       <c r="U59" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V59" s="1" t="n">
-        <v>0.5889727405753026</v>
+      <c r="V59" t="n">
+        <v>0.6035174675167421</v>
       </c>
     </row>
     <row r="60">
@@ -4492,7 +4492,7 @@
         <v>-0.1767330850873675</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>2.998803481508547</v>
+        <v>3</v>
       </c>
       <c r="D60" t="n">
         <v>6</v>
@@ -4507,7 +4507,7 @@
         <v>1</v>
       </c>
       <c r="H60" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I60" t="n">
         <v>0.1041666666666667</v>
@@ -4533,8 +4533,8 @@
       <c r="P60" t="n">
         <v>0.5371926654867829</v>
       </c>
-      <c r="Q60" s="1" t="n">
-        <v>6</v>
+      <c r="Q60" t="n">
+        <v>4</v>
       </c>
       <c r="R60" t="n">
         <v>1.714203171343286</v>
@@ -4548,8 +4548,8 @@
       <c r="U60" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V60" s="1" t="n">
-        <v>0.7519781333833444</v>
+      <c r="V60" t="n">
+        <v>0.7705482909857329</v>
       </c>
     </row>
     <row r="61">
@@ -4560,7 +4560,7 @@
         <v>-0.4562288522720337</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>1.837308766502761</v>
+        <v>2</v>
       </c>
       <c r="D61" t="n">
         <v>6</v>
@@ -4574,8 +4574,8 @@
       <c r="G61" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H61" s="1" t="n">
-        <v>5</v>
+      <c r="H61" t="n">
+        <v>4</v>
       </c>
       <c r="I61" t="n">
         <v>0.03401360544217687</v>
@@ -4601,8 +4601,8 @@
       <c r="P61" t="n">
         <v>0.2440544779975879</v>
       </c>
-      <c r="Q61" s="1" t="n">
-        <v>4</v>
+      <c r="Q61" t="n">
+        <v>5</v>
       </c>
       <c r="R61" t="n">
         <v>1.885299500946812</v>
@@ -4616,8 +4616,8 @@
       <c r="U61" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V61" s="1" t="n">
-        <v>0.8507203206479008</v>
+      <c r="V61" t="n">
+        <v>0.8717289241280402</v>
       </c>
     </row>
     <row r="62">
@@ -4628,7 +4628,7 @@
         <v>-1.379035830497742</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>3.095129001670651</v>
+        <v>4</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>10</v>
@@ -4642,8 +4642,8 @@
       <c r="G62" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H62" s="1" t="n">
-        <v>6</v>
+      <c r="H62" t="n">
+        <v>13</v>
       </c>
       <c r="I62" t="n">
         <v>0.1111111111111111</v>
@@ -4669,8 +4669,8 @@
       <c r="P62" t="n">
         <v>0.8388125180040888</v>
       </c>
-      <c r="Q62" s="1" t="n">
-        <v>13</v>
+      <c r="Q62" t="n">
+        <v>6</v>
       </c>
       <c r="R62" t="n">
         <v>1.483611654966423</v>
@@ -4684,8 +4684,8 @@
       <c r="U62" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V62" s="1" t="n">
-        <v>0.6376839124264988</v>
+      <c r="V62" t="n">
+        <v>0.6534315654878825</v>
       </c>
     </row>
     <row r="63">
@@ -4696,7 +4696,7 @@
         <v>1.000827193260193</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>3.68480070840787</v>
+        <v>4</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>8</v>
@@ -4710,8 +4710,8 @@
       <c r="G63" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H63" s="1" t="n">
-        <v>5</v>
+      <c r="H63" t="n">
+        <v>15</v>
       </c>
       <c r="I63" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -4737,8 +4737,8 @@
       <c r="P63" t="n">
         <v>0.7348060490043172</v>
       </c>
-      <c r="Q63" s="1" t="n">
-        <v>15</v>
+      <c r="Q63" t="n">
+        <v>5</v>
       </c>
       <c r="R63" t="n">
         <v>1.73023804570537</v>
@@ -4752,8 +4752,8 @@
       <c r="U63" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V63" s="1" t="n">
-        <v>0.6135343276114881</v>
+      <c r="V63" t="n">
+        <v>0.6286856048261045</v>
       </c>
     </row>
     <row r="64">
@@ -4764,7 +4764,7 @@
         <v>1.074292063713074</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>2.907311151616438</v>
+        <v>4</v>
       </c>
       <c r="D64" t="n">
         <v>7</v>
@@ -4778,8 +4778,8 @@
       <c r="G64" t="n">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H64" s="1" t="n">
-        <v>6</v>
+      <c r="H64" t="n">
+        <v>15</v>
       </c>
       <c r="I64" t="n">
         <v>0.0625</v>
@@ -4805,8 +4805,8 @@
       <c r="P64" t="n">
         <v>0.6688431671727501</v>
       </c>
-      <c r="Q64" s="1" t="n">
-        <v>15</v>
+      <c r="Q64" t="n">
+        <v>6</v>
       </c>
       <c r="R64" t="n">
         <v>1.73023804570537</v>
@@ -4820,8 +4820,8 @@
       <c r="U64" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V64" s="1" t="n">
-        <v>0.7125797158656658</v>
+      <c r="V64" t="n">
+        <v>0.7301769265296958</v>
       </c>
     </row>
     <row r="65">
@@ -4832,7 +4832,7 @@
         <v>0.8525265455245972</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>3.285859775952992</v>
+        <v>4</v>
       </c>
       <c r="D65" t="n">
         <v>8</v>
@@ -4846,8 +4846,8 @@
       <c r="G65" t="n">
         <v>1</v>
       </c>
-      <c r="H65" s="1" t="n">
-        <v>5</v>
+      <c r="H65" t="n">
+        <v>12</v>
       </c>
       <c r="I65" t="n">
         <v>0.1111111111111111</v>
@@ -4873,8 +4873,8 @@
       <c r="P65" t="n">
         <v>0.728706648937482</v>
       </c>
-      <c r="Q65" s="1" t="n">
-        <v>12</v>
+      <c r="Q65" t="n">
+        <v>5</v>
       </c>
       <c r="R65" s="1" t="n">
         <v>1.665693703666284</v>
@@ -4888,8 +4888,8 @@
       <c r="U65" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V65" s="1" t="n">
-        <v>0.6997252821898771</v>
+      <c r="V65" t="n">
+        <v>0.7170050516296856</v>
       </c>
     </row>
     <row r="66">
@@ -4900,7 +4900,7 @@
         <v>0.7601801753044128</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>3.238479202448134</v>
+        <v>4</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>8</v>
@@ -4914,8 +4914,8 @@
       <c r="G66" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H66" s="1" t="n">
-        <v>7</v>
+      <c r="H66" t="n">
+        <v>16</v>
       </c>
       <c r="I66" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -4941,8 +4941,8 @@
       <c r="P66" t="n">
         <v>0.7478701909544907</v>
       </c>
-      <c r="Q66" s="1" t="n">
-        <v>16</v>
+      <c r="Q66" t="n">
+        <v>7</v>
       </c>
       <c r="R66" t="n">
         <v>1.73023804570537</v>
@@ -4956,8 +4956,8 @@
       <c r="U66" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V66" s="1" t="n">
-        <v>0.6442363093792414</v>
+      <c r="V66" t="n">
+        <v>0.6601457743852601</v>
       </c>
     </row>
     <row r="67">
@@ -4968,7 +4968,7 @@
         <v>-1.36204195022583</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>3.312365901246937</v>
+        <v>4</v>
       </c>
       <c r="D67" t="n">
         <v>9</v>
@@ -4983,7 +4983,7 @@
         <v>0.9130434782608695</v>
       </c>
       <c r="H67" s="1" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I67" t="n">
         <v>0.1111111111111111</v>
@@ -5009,8 +5009,8 @@
       <c r="P67" t="n">
         <v>0.812657865345757</v>
       </c>
-      <c r="Q67" s="1" t="n">
-        <v>15</v>
+      <c r="Q67" t="n">
+        <v>6</v>
       </c>
       <c r="R67" t="n">
         <v>1.665693703666284</v>
@@ -5024,8 +5024,8 @@
       <c r="U67" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V67" s="1" t="n">
-        <v>0.6439677083574314</v>
+      <c r="V67" t="n">
+        <v>0.6598705402406428</v>
       </c>
     </row>
     <row r="68">
@@ -5036,7 +5036,7 @@
         <v>-0.7230163812637329</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>1.83486141245687</v>
+        <v>2</v>
       </c>
       <c r="D68" t="n">
         <v>6</v>
@@ -5092,8 +5092,8 @@
       <c r="U68" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V68" s="1" t="n">
-        <v>0.9414478639673471</v>
+      <c r="V68" t="n">
+        <v>0.9646969910791235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed sb_mean and sb_diff
</commit_message>
<xml_diff>
--- a/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
+++ b/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
@@ -698,8 +698,8 @@
       <c r="G4" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H4" s="1" t="n">
-        <v>4</v>
+      <c r="H4" t="n">
+        <v>3</v>
       </c>
       <c r="I4" t="n">
         <v>0.03401360544217687</v>
@@ -1310,8 +1310,8 @@
       <c r="G13" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H13" s="1" t="n">
-        <v>17</v>
+      <c r="H13" t="n">
+        <v>16</v>
       </c>
       <c r="I13" t="n">
         <v>0.1111111111111111</v>
@@ -1446,8 +1446,8 @@
       <c r="G15" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H15" s="1" t="n">
-        <v>16</v>
+      <c r="H15" t="n">
+        <v>15</v>
       </c>
       <c r="I15" t="n">
         <v>0.1111111111111111</v>
@@ -1514,8 +1514,8 @@
       <c r="G16" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H16" s="1" t="n">
-        <v>16</v>
+      <c r="H16" t="n">
+        <v>15</v>
       </c>
       <c r="I16" t="n">
         <v>0.1111111111111111</v>
@@ -1650,8 +1650,8 @@
       <c r="G18" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H18" s="1" t="n">
-        <v>8</v>
+      <c r="H18" t="n">
+        <v>7</v>
       </c>
       <c r="I18" t="n">
         <v>0.1111111111111111</v>
@@ -1718,8 +1718,8 @@
       <c r="G19" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H19" s="1" t="n">
-        <v>7</v>
+      <c r="H19" t="n">
+        <v>6</v>
       </c>
       <c r="I19" t="n">
         <v>0.1666666666666667</v>
@@ -1786,8 +1786,8 @@
       <c r="G20" t="n">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H20" s="1" t="n">
-        <v>16</v>
+      <c r="H20" t="n">
+        <v>15</v>
       </c>
       <c r="I20" t="n">
         <v>0.1111111111111111</v>
@@ -1990,8 +1990,8 @@
       <c r="G23" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H23" s="1" t="n">
-        <v>16</v>
+      <c r="H23" t="n">
+        <v>15</v>
       </c>
       <c r="I23" t="n">
         <v>0.1111111111111111</v>
@@ -2058,8 +2058,8 @@
       <c r="G24" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H24" s="1" t="n">
-        <v>17</v>
+      <c r="H24" t="n">
+        <v>16</v>
       </c>
       <c r="I24" t="n">
         <v>0.1111111111111111</v>
@@ -2126,8 +2126,8 @@
       <c r="G25" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H25" s="1" t="n">
-        <v>16</v>
+      <c r="H25" t="n">
+        <v>15</v>
       </c>
       <c r="I25" t="n">
         <v>0.1111111111111111</v>
@@ -2466,8 +2466,8 @@
       <c r="G30" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H30" s="1" t="n">
-        <v>16</v>
+      <c r="H30" t="n">
+        <v>15</v>
       </c>
       <c r="I30" t="n">
         <v>0.1111111111111111</v>
@@ -2534,8 +2534,8 @@
       <c r="G31" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H31" s="1" t="n">
-        <v>16</v>
+      <c r="H31" t="n">
+        <v>15</v>
       </c>
       <c r="I31" t="n">
         <v>0.1111111111111111</v>
@@ -2806,8 +2806,8 @@
       <c r="G35" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H35" s="1" t="n">
-        <v>7</v>
+      <c r="H35" t="n">
+        <v>6</v>
       </c>
       <c r="I35" t="n">
         <v>0.1111111111111111</v>
@@ -2942,8 +2942,8 @@
       <c r="G37" t="n">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H37" s="1" t="n">
-        <v>16</v>
+      <c r="H37" t="n">
+        <v>15</v>
       </c>
       <c r="I37" t="n">
         <v>0.1111111111111111</v>
@@ -3146,8 +3146,8 @@
       <c r="G40" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H40" s="1" t="n">
-        <v>16</v>
+      <c r="H40" t="n">
+        <v>15</v>
       </c>
       <c r="I40" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -3418,8 +3418,8 @@
       <c r="G44" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H44" s="1" t="n">
-        <v>16</v>
+      <c r="H44" t="n">
+        <v>15</v>
       </c>
       <c r="I44" t="n">
         <v>0.1111111111111111</v>
@@ -3758,8 +3758,8 @@
       <c r="G49" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H49" s="1" t="n">
-        <v>16</v>
+      <c r="H49" t="n">
+        <v>15</v>
       </c>
       <c r="I49" t="n">
         <v>0.1111111111111111</v>
@@ -3962,8 +3962,8 @@
       <c r="G52" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H52" s="1" t="n">
-        <v>16</v>
+      <c r="H52" t="n">
+        <v>15</v>
       </c>
       <c r="I52" s="1" t="n">
         <v>0.1111111111111111</v>
@@ -4098,8 +4098,8 @@
       <c r="G54" t="n">
         <v>1</v>
       </c>
-      <c r="H54" s="1" t="n">
-        <v>16</v>
+      <c r="H54" t="n">
+        <v>15</v>
       </c>
       <c r="I54" t="n">
         <v>0.1111111111111111</v>
@@ -4370,8 +4370,8 @@
       <c r="G58" t="n">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H58" s="1" t="n">
-        <v>16</v>
+      <c r="H58" t="n">
+        <v>15</v>
       </c>
       <c r="I58" t="n">
         <v>0.1111111111111111</v>
@@ -4506,8 +4506,8 @@
       <c r="G60" t="n">
         <v>1</v>
       </c>
-      <c r="H60" s="1" t="n">
-        <v>6</v>
+      <c r="H60" t="n">
+        <v>5</v>
       </c>
       <c r="I60" t="n">
         <v>0.1041666666666667</v>
@@ -4982,8 +4982,8 @@
       <c r="G67" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H67" s="1" t="n">
-        <v>15</v>
+      <c r="H67" t="n">
+        <v>14</v>
       </c>
       <c r="I67" t="n">
         <v>0.1111111111111111</v>

</xml_diff>

<commit_message>
fixed catch22 code quality
</commit_message>
<xml_diff>
--- a/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
+++ b/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
@@ -26,12 +26,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -424,112 +431,112 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>DN_HistogramMode_5</t>
+          <t>mode_5</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>DN_HistogramMode_10</t>
+          <t>mode_10</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>CO_f1ecac</t>
+          <t>stretch_high</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>CO_FirstMin_ac</t>
+          <t>outlier_timing_pos</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>CO_HistogramAMI_even_2_5</t>
+          <t>outlier_timing_neg</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>CO_trev_1_num</t>
+          <t>acf_timescale</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>MD_hrv_classic_pnn40</t>
+          <t>acf_first_min</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>SB_BinaryStats_mean_longstretch1</t>
+          <t>centroid_freq</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>SB_TransitionMatrix_3ac_sumdiagcov</t>
+          <t>low_freq_power</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>PD_PeriodicityWang_th0_01</t>
+          <t>forecast_error</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>CO_Embed2_Dist_tau_d_expfit_meandiff</t>
+          <t>trev</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>IN_AutoMutualInfoStats_40_gaussian_fmmi</t>
+          <t>ami2</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>FC_LocalSimple_mean1_tauresrat</t>
+          <t>ami_timescale</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>DN_OutlierInclude_p_001_mdrmd</t>
+          <t>high_fluctuation</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>DN_OutlierInclude_n_001_mdrmd</t>
+          <t>stretch_decreasing</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>SP_Summaries_welch_rect_area_5_1</t>
+          <t>entropy_pairs</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>SB_BinaryStats_diff_longstretch0</t>
+          <t>whiten_timescale</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>SB_MotifThree_quantile_hh</t>
+          <t>periodicity</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>SC_FluctAnal_2_rsrangefit_50_1_logi_prop_r1</t>
+          <t>dfa</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>SC_FluctAnal_2_dfa_50_1_2_logi_prop_r1</t>
+          <t>rs_range</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>SP_Summaries_welch_rect_centroid</t>
+          <t>transition_matrix</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>FC_LocalSimple_mean3_stderr</t>
+          <t>periodicity</t>
         </is>
       </c>
     </row>
@@ -597,8 +604,8 @@
       <c r="U2" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V2" t="n">
-        <v>0.8574191573061893</v>
+      <c r="V2" s="1" t="n">
+        <v>1.787502084491367</v>
       </c>
     </row>
     <row r="3">
@@ -665,8 +672,8 @@
       <c r="U3" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V3" t="n">
-        <v>0.6826107272137758</v>
+      <c r="V3" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="4">
@@ -733,8 +740,8 @@
       <c r="U4" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V4" t="n">
-        <v>0.8864360551857</v>
+      <c r="V4" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="5">
@@ -801,8 +808,8 @@
       <c r="U5" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V5" t="n">
-        <v>0.6643191885375342</v>
+      <c r="V5" s="1" t="n">
+        <v>1.605420035791506</v>
       </c>
     </row>
     <row r="6">
@@ -869,8 +876,8 @@
       <c r="U6" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V6" t="n">
-        <v>0.6741940111567349</v>
+      <c r="V6" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="7">
@@ -937,8 +944,8 @@
       <c r="U7" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V7" t="n">
-        <v>0.8184240915298243</v>
+      <c r="V7" s="1" t="n">
+        <v>1.778747513382372</v>
       </c>
     </row>
     <row r="8">
@@ -1005,8 +1012,8 @@
       <c r="U8" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V8" t="n">
-        <v>0.8883513367359682</v>
+      <c r="V8" s="1" t="n">
+        <v>1.847775752366145</v>
       </c>
     </row>
     <row r="9">
@@ -1073,8 +1080,8 @@
       <c r="U9" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V9" t="n">
-        <v>0.6289793636448475</v>
+      <c r="V9" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="10">
@@ -1141,8 +1148,8 @@
       <c r="U10" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V10" t="n">
-        <v>0.6154088878652204</v>
+      <c r="V10" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="11">
@@ -1209,8 +1216,8 @@
       <c r="U11" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V11" t="n">
-        <v>0.6682353638799723</v>
+      <c r="V11" s="1" t="n">
+        <v>1.483611654966423</v>
       </c>
     </row>
     <row r="12">
@@ -1277,8 +1284,8 @@
       <c r="U12" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V12" t="n">
-        <v>0.7552580635694194</v>
+      <c r="V12" s="1" t="n">
+        <v>1.911059049329703</v>
       </c>
     </row>
     <row r="13">
@@ -1345,8 +1352,8 @@
       <c r="U13" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V13" t="n">
-        <v>0.7156207708092244</v>
+      <c r="V13" s="1" t="n">
+        <v>1.790511713580147</v>
       </c>
     </row>
     <row r="14">
@@ -1413,8 +1420,8 @@
       <c r="U14" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V14" t="n">
-        <v>0.6814319447688442</v>
+      <c r="V14" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="15">
@@ -1481,8 +1488,8 @@
       <c r="U15" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V15" t="n">
-        <v>0.65708644925339</v>
+      <c r="V15" s="1" t="n">
+        <v>1.665693703666284</v>
       </c>
     </row>
     <row r="16">
@@ -1549,8 +1556,8 @@
       <c r="U16" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V16" t="n">
-        <v>0.6849799384292986</v>
+      <c r="V16" s="1" t="n">
+        <v>1.730238045705369</v>
       </c>
     </row>
     <row r="17">
@@ -1617,8 +1624,8 @@
       <c r="U17" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V17" t="n">
-        <v>0.7670002264041113</v>
+      <c r="V17" s="1" t="n">
+        <v>1.819976677806285</v>
       </c>
     </row>
     <row r="18">
@@ -1685,8 +1692,8 @@
       <c r="U18" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V18" t="n">
-        <v>0.7218312500339272</v>
+      <c r="V18" s="1" t="n">
+        <v>1.778747513382372</v>
       </c>
     </row>
     <row r="19">
@@ -1753,8 +1760,8 @@
       <c r="U19" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V19" t="n">
-        <v>0.7055351163517595</v>
+      <c r="V19" s="1" t="n">
+        <v>1.714203171343286</v>
       </c>
     </row>
     <row r="20">
@@ -1821,8 +1828,8 @@
       <c r="U20" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V20" t="n">
-        <v>0.6458425355632602</v>
+      <c r="V20" s="1" t="n">
+        <v>1.483611654966423</v>
       </c>
     </row>
     <row r="21">
@@ -1889,8 +1896,8 @@
       <c r="U21" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V21" t="n">
-        <v>0.6492256208314514</v>
+      <c r="V21" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="22">
@@ -1957,8 +1964,8 @@
       <c r="U22" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V22" t="n">
-        <v>0.667185686402688</v>
+      <c r="V22" s="1" t="n">
+        <v>1.790511713580147</v>
       </c>
     </row>
     <row r="23">
@@ -2025,8 +2032,8 @@
       <c r="U23" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V23" t="n">
-        <v>0.6662215934181749</v>
+      <c r="V23" s="1" t="n">
+        <v>1.483611654966423</v>
       </c>
     </row>
     <row r="24">
@@ -2093,8 +2100,8 @@
       <c r="U24" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V24" t="n">
-        <v>0.6798841218158759</v>
+      <c r="V24" s="1" t="n">
+        <v>1.790511713580147</v>
       </c>
     </row>
     <row r="25">
@@ -2161,8 +2168,8 @@
       <c r="U25" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V25" t="n">
-        <v>0.6999238317103339</v>
+      <c r="V25" s="1" t="n">
+        <v>1.605420035791506</v>
       </c>
     </row>
     <row r="26">
@@ -2229,8 +2236,8 @@
       <c r="U26" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V26" t="n">
-        <v>0.7066769666510576</v>
+      <c r="V26" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="27">
@@ -2297,8 +2304,8 @@
       <c r="U27" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V27" t="n">
-        <v>0.9299716493102558</v>
+      <c r="V27" s="1" t="n">
+        <v>1.83902118125715</v>
       </c>
     </row>
     <row r="28">
@@ -2365,8 +2372,8 @@
       <c r="U28" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V28" t="n">
-        <v>0.7012995687514046</v>
+      <c r="V28" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="29">
@@ -2433,8 +2440,8 @@
       <c r="U29" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V29" t="n">
-        <v>0.6754997567266193</v>
+      <c r="V29" s="1" t="n">
+        <v>1.714203171343286</v>
       </c>
     </row>
     <row r="30">
@@ -2501,8 +2508,8 @@
       <c r="U30" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V30" t="n">
-        <v>0.651422242259642</v>
+      <c r="V30" s="1" t="n">
+        <v>1.605420035791506</v>
       </c>
     </row>
     <row r="31">
@@ -2569,8 +2576,8 @@
       <c r="U31" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V31" t="n">
-        <v>0.6858122216291865</v>
+      <c r="V31" s="1" t="n">
+        <v>1.665693703666284</v>
       </c>
     </row>
     <row r="32">
@@ -2637,8 +2644,8 @@
       <c r="U32" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V32" t="n">
-        <v>0.6561863467065937</v>
+      <c r="V32" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="33">
@@ -2705,8 +2712,8 @@
       <c r="U33" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V33" t="n">
-        <v>0.8376587367987973</v>
+      <c r="V33" s="1" t="n">
+        <v>1.885299500946812</v>
       </c>
     </row>
     <row r="34">
@@ -2773,8 +2780,8 @@
       <c r="U34" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V34" t="n">
-        <v>0.6516400889749291</v>
+      <c r="V34" s="1" t="n">
+        <v>1.483611654966423</v>
       </c>
     </row>
     <row r="35">
@@ -2841,8 +2848,8 @@
       <c r="U35" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V35" t="n">
-        <v>0.7400365745078062</v>
+      <c r="V35" s="1" t="n">
+        <v>1.714203171343286</v>
       </c>
     </row>
     <row r="36">
@@ -2909,8 +2916,8 @@
       <c r="U36" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V36" t="n">
-        <v>0.8960191792551805</v>
+      <c r="V36" s="1" t="n">
+        <v>1.994082636498592</v>
       </c>
     </row>
     <row r="37">
@@ -2977,8 +2984,8 @@
       <c r="U37" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V37" t="n">
-        <v>0.6446974682455934</v>
+      <c r="V37" s="1" t="n">
+        <v>1.605420035791506</v>
       </c>
     </row>
     <row r="38">
@@ -3045,8 +3052,8 @@
       <c r="U38" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V38" t="n">
-        <v>0.6012963197891809</v>
+      <c r="V38" s="1" t="n">
+        <v>1.790511713580147</v>
       </c>
     </row>
     <row r="39">
@@ -3113,8 +3120,8 @@
       <c r="U39" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V39" t="n">
-        <v>0.9560072040126173</v>
+      <c r="V39" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="40">
@@ -3181,8 +3188,8 @@
       <c r="U40" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V40" t="n">
-        <v>0.6640850982452019</v>
+      <c r="V40" s="1" t="n">
+        <v>1.665693703666284</v>
       </c>
     </row>
     <row r="41">
@@ -3249,8 +3256,8 @@
       <c r="U41" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V41" t="n">
-        <v>0.6046829025695121</v>
+      <c r="V41" s="1" t="n">
+        <v>1.605420035791506</v>
       </c>
     </row>
     <row r="42">
@@ -3317,8 +3324,8 @@
       <c r="U42" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V42" t="n">
-        <v>0.847826137624116</v>
+      <c r="V42" s="1" t="n">
+        <v>1.714203171343286</v>
       </c>
     </row>
     <row r="43">
@@ -3385,8 +3392,8 @@
       <c r="U43" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V43" t="n">
-        <v>0.7073200176862909</v>
+      <c r="V43" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="44">
@@ -3453,8 +3460,8 @@
       <c r="U44" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V44" t="n">
-        <v>0.6199724495025251</v>
+      <c r="V44" s="1" t="n">
+        <v>1.483611654966423</v>
       </c>
     </row>
     <row r="45">
@@ -3521,8 +3528,8 @@
       <c r="U45" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V45" t="n">
-        <v>0.8716415822789345</v>
+      <c r="V45" s="1" t="n">
+        <v>1.834750507092842</v>
       </c>
     </row>
     <row r="46">
@@ -3589,8 +3596,8 @@
       <c r="U46" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V46" t="n">
-        <v>0.6827214533705925</v>
+      <c r="V46" s="1" t="n">
+        <v>1.730238045705369</v>
       </c>
     </row>
     <row r="47">
@@ -3657,8 +3664,8 @@
       <c r="U47" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V47" t="n">
-        <v>0.6704933583602372</v>
+      <c r="V47" s="1" t="n">
+        <v>1.483611654966423</v>
       </c>
     </row>
     <row r="48">
@@ -3725,8 +3732,8 @@
       <c r="U48" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V48" t="n">
-        <v>0.8476026266696666</v>
+      <c r="V48" s="1" t="n">
+        <v>1.836011552168369</v>
       </c>
     </row>
     <row r="49">
@@ -3793,8 +3800,8 @@
       <c r="U49" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V49" t="n">
-        <v>0.6430829873760525</v>
+      <c r="V49" s="1" t="n">
+        <v>1.483611654966423</v>
       </c>
     </row>
     <row r="50">
@@ -3861,8 +3868,8 @@
       <c r="U50" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V50" t="n">
-        <v>0.7987267666407276</v>
+      <c r="V50" s="1" t="n">
+        <v>1.751726919923953</v>
       </c>
     </row>
     <row r="51">
@@ -3929,8 +3936,8 @@
       <c r="U51" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V51" t="n">
-        <v>0.9354075367230528</v>
+      <c r="V51" s="1" t="n">
+        <v>1.548155997005509</v>
       </c>
     </row>
     <row r="52">
@@ -3997,8 +4004,8 @@
       <c r="U52" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V52" t="n">
-        <v>0.6836890455803701</v>
+      <c r="V52" s="1" t="n">
+        <v>1.548155997005509</v>
       </c>
     </row>
     <row r="53">
@@ -4065,8 +4072,8 @@
       <c r="U53" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V53" t="n">
-        <v>0.8369230021690024</v>
+      <c r="V53" s="1" t="n">
+        <v>1.665693703666284</v>
       </c>
     </row>
     <row r="54">
@@ -4133,8 +4140,8 @@
       <c r="U54" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V54" t="n">
-        <v>0.6445781827085135</v>
+      <c r="V54" s="1" t="n">
+        <v>1.639934155283393</v>
       </c>
     </row>
     <row r="55">
@@ -4201,8 +4208,8 @@
       <c r="U55" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V55" t="n">
-        <v>0.9339964139920454</v>
+      <c r="V55" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="56">
@@ -4269,8 +4276,8 @@
       <c r="U56" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V56" t="n">
-        <v>0.907844931347941</v>
+      <c r="V56" s="1" t="n">
+        <v>1.816271261963039</v>
       </c>
     </row>
     <row r="57">
@@ -4337,8 +4344,8 @@
       <c r="U57" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V57" t="n">
-        <v>0.6487154681166755</v>
+      <c r="V57" s="1" t="n">
+        <v>1.790511713580147</v>
       </c>
     </row>
     <row r="58">
@@ -4405,8 +4412,8 @@
       <c r="U58" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V58" t="n">
-        <v>0.6611991176085891</v>
+      <c r="V58" s="1" t="n">
+        <v>1.665693703666284</v>
       </c>
     </row>
     <row r="59">
@@ -4473,8 +4480,8 @@
       <c r="U59" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V59" t="n">
-        <v>0.6035174675167421</v>
+      <c r="V59" s="1" t="n">
+        <v>1.790511713580147</v>
       </c>
     </row>
     <row r="60">
@@ -4541,8 +4548,8 @@
       <c r="U60" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V60" t="n">
-        <v>0.7705482909857329</v>
+      <c r="V60" s="1" t="n">
+        <v>1.714203171343286</v>
       </c>
     </row>
     <row r="61">
@@ -4609,8 +4616,8 @@
       <c r="U61" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V61" t="n">
-        <v>0.8717289241280402</v>
+      <c r="V61" s="1" t="n">
+        <v>1.885299500946812</v>
       </c>
     </row>
     <row r="62">
@@ -4677,8 +4684,8 @@
       <c r="U62" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V62" t="n">
-        <v>0.6534315654878825</v>
+      <c r="V62" s="1" t="n">
+        <v>1.483611654966423</v>
       </c>
     </row>
     <row r="63">
@@ -4745,8 +4752,8 @@
       <c r="U63" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V63" t="n">
-        <v>0.6286856048261045</v>
+      <c r="V63" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="64">
@@ -4813,8 +4820,8 @@
       <c r="U64" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V64" t="n">
-        <v>0.7301769265296958</v>
+      <c r="V64" s="1" t="n">
+        <v>1.730238045705369</v>
       </c>
     </row>
     <row r="65">
@@ -4881,8 +4888,8 @@
       <c r="U65" t="n">
         <v>0.3926990816987241</v>
       </c>
-      <c r="V65" t="n">
-        <v>0.7170050516296856</v>
+      <c r="V65" s="1" t="n">
+        <v>1.857500426386953</v>
       </c>
     </row>
     <row r="66">
@@ -4949,8 +4956,8 @@
       <c r="U66" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V66" t="n">
-        <v>0.6601457743852601</v>
+      <c r="V66" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
     </row>
     <row r="67">
@@ -5017,8 +5024,8 @@
       <c r="U67" t="n">
         <v>0.1963495408493621</v>
       </c>
-      <c r="V67" t="n">
-        <v>0.6598705402406428</v>
+      <c r="V67" s="1" t="n">
+        <v>1.665693703666284</v>
       </c>
     </row>
     <row r="68">
@@ -5085,8 +5092,8 @@
       <c r="U68" t="n">
         <v>0.5890486225480862</v>
       </c>
-      <c r="V68" t="n">
-        <v>0.9646969910791235</v>
+      <c r="V68" s="1" t="n">
+        <v>1.831740878004061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>